<commit_message>
expenses for 3rd and 4th
</commit_message>
<xml_diff>
--- a/DailyExpenditure.xlsx
+++ b/DailyExpenditure.xlsx
@@ -6906,7 +6906,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="63">
   <si>
     <t>DATE</t>
   </si>
@@ -6941,16 +6941,13 @@
     <t>IN HAND</t>
   </si>
   <si>
-    <t>RETURN </t>
+    <t>RETURN</t>
   </si>
   <si>
-    <t>EXPECTED </t>
+    <t>EXPECTED</t>
   </si>
   <si>
     <t>SALARY</t>
-  </si>
-  <si>
-    <t> </t>
   </si>
   <si>
     <t>EXPECTED OTHER EXP</t>
@@ -7016,7 +7013,7 @@
     <t>Thodupuzha mrg    exp 300</t>
   </si>
   <si>
-    <t>To hm </t>
+    <t>To hm</t>
   </si>
   <si>
     <t>Trigil</t>
@@ -7028,7 +7025,7 @@
     <t>To-Sadam</t>
   </si>
   <si>
-    <t>To-Trigil </t>
+    <t>To-Trigil</t>
   </si>
   <si>
     <t>BIKE-PETROL</t>
@@ -7055,7 +7052,7 @@
     <t>Total To JP 11000</t>
   </si>
   <si>
-    <t>inhand </t>
+    <t>inhand</t>
   </si>
   <si>
     <t>debt</t>
@@ -7377,7 +7374,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7415,10 +7412,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="6" borderId="2" xfId="24" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7510,10 +7503,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7526,13 +7515,13 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Note" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Good" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Calculation" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Input" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Note" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Good" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Bad" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Neutral" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Calculation" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Input" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Check Cell" xfId="26" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -7605,7 +7594,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L23" activeCellId="0" sqref="L23"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7699,9 +7688,12 @@
       <c r="D3" s="0" t="n">
         <v>218</v>
       </c>
+      <c r="G3" s="0" t="n">
+        <v>177</v>
+      </c>
       <c r="I3" s="2" t="n">
         <f aca="false">SUM(B3,C3,D3,E3,F3,G3)</f>
-        <v>913</v>
+        <v>1090</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>11</v>
@@ -7714,9 +7706,15 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>340</v>
+      </c>
       <c r="I4" s="2" t="n">
         <f aca="false">SUM(B4,C4,D4,E4,F4,G4)</f>
-        <v>0</v>
+        <v>370</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>12</v>
@@ -7761,9 +7759,7 @@
         <f aca="false">SUM(B7,C7,D7,E7,F7,G7)</f>
         <v>0</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="K7" s="4"/>
       <c r="L7" s="5"/>
       <c r="M7" s="4"/>
       <c r="N7" s="6"/>
@@ -7859,7 +7855,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L16" s="7"/>
     </row>
@@ -7872,7 +7868,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L17" s="9" t="n">
         <v>15000</v>
@@ -7887,7 +7883,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L18" s="9"/>
     </row>
@@ -7900,7 +7896,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L19" s="9"/>
     </row>
@@ -7939,7 +7935,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L22" s="9" t="n">
         <v>2000</v>
@@ -7954,7 +7950,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L23" s="9" t="n">
         <v>1000</v>
@@ -7969,7 +7965,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L24" s="9"/>
     </row>
@@ -7982,7 +7978,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L25" s="9"/>
     </row>
@@ -8045,8 +8041,6 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="D31" s="10"/>
       <c r="I31" s="2" t="n">
         <f aca="false">SUM(B31,C31,D31,E31,F31,G31)</f>
         <v>0</v>
@@ -8066,104 +8060,100 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="10"/>
-      <c r="D33" s="10"/>
-    </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>160</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>695</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
-        <v>567</v>
-      </c>
-      <c r="E34" s="12" t="n">
+        <v>597</v>
+      </c>
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>379</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F33)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(G2:G32)</f>
-        <v>15000</v>
-      </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14" t="n">
+        <v>15517</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34)</f>
-        <v>16801</v>
+        <v>17348</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1500</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>4300</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>300</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <f aca="false">SUM(L17:L30)</f>
         <v>22000</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14" t="n">
+      <c r="H35" s="12"/>
+      <c r="I35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35)</f>
         <v>30100</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>1340</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>3605</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
-        <v>433</v>
-      </c>
-      <c r="E36" s="18" t="n">
+        <v>403</v>
+      </c>
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>621</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>300</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
-        <v>7000</v>
-      </c>
-      <c r="I36" s="18" t="n">
+        <v>6483</v>
+      </c>
+      <c r="I36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36)</f>
-        <v>13299</v>
+        <v>12752</v>
       </c>
     </row>
   </sheetData>
@@ -8221,7 +8211,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -8238,8 +8228,8 @@
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="27" t="s">
-        <v>57</v>
+      <c r="M1" s="26" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8263,7 +8253,7 @@
         <f aca="false">SUM(B2,C2,D2,E2,F2,G2,H2)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="27" t="n">
+      <c r="M2" s="26" t="n">
         <v>1152</v>
       </c>
     </row>
@@ -8290,7 +8280,7 @@
         <f aca="false">SUM(B3,C3,D3,E3,F3,G3,H3)</f>
         <v>1994</v>
       </c>
-      <c r="M3" s="27" t="n">
+      <c r="M3" s="26" t="n">
         <v>1994</v>
       </c>
     </row>
@@ -8313,7 +8303,7 @@
         <f aca="false">SUM(B4,C4,D4,E4,F4,G4,H4)</f>
         <v>154</v>
       </c>
-      <c r="M4" s="27"/>
+      <c r="M4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -8383,7 +8373,7 @@
         <v>60</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8425,7 +8415,7 @@
         <f aca="false">SUM(B9,C9,D9,E9,F9,G9,H9)</f>
         <v>928</v>
       </c>
-      <c r="N9" s="31" t="n">
+      <c r="N9" s="30" t="n">
         <v>463</v>
       </c>
     </row>
@@ -8450,7 +8440,7 @@
         <f aca="false">SUM(B10,C10,D10,E10,F10,G10,H10)</f>
         <v>548</v>
       </c>
-      <c r="N10" s="31" t="n">
+      <c r="N10" s="30" t="n">
         <v>165</v>
       </c>
     </row>
@@ -8473,7 +8463,7 @@
         <f aca="false">SUM(B11,C11,D11,E11,F11,G11,H11)</f>
         <v>936</v>
       </c>
-      <c r="N11" s="31" t="n">
+      <c r="N11" s="30" t="n">
         <v>780</v>
       </c>
     </row>
@@ -8496,7 +8486,7 @@
         <f aca="false">SUM(B12,C12,D12,E12,F12,G12,H12)</f>
         <v>67</v>
       </c>
-      <c r="N12" s="31"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -8517,7 +8507,7 @@
         <f aca="false">SUM(B13,C13,D13,E13,F13,G13,H13)</f>
         <v>1234</v>
       </c>
-      <c r="N13" s="31"/>
+      <c r="N13" s="30"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -8536,7 +8526,7 @@
         <f aca="false">SUM(B14,C14,D14,E14,F14,G14,H14)</f>
         <v>0</v>
       </c>
-      <c r="N14" s="31"/>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -8559,7 +8549,7 @@
         <f aca="false">SUM(B15,C15,D15,E15,F15,G15,H15)</f>
         <v>1254</v>
       </c>
-      <c r="N15" s="31"/>
+      <c r="N15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -8580,7 +8570,7 @@
         <f aca="false">SUM(B16,C16,D16,E16,F16,G16,H16)</f>
         <v>99</v>
       </c>
-      <c r="N16" s="31"/>
+      <c r="N16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -8601,7 +8591,7 @@
         <f aca="false">SUM(B17,C17,D17,E17,F17,G17,H17)</f>
         <v>223</v>
       </c>
-      <c r="N17" s="31"/>
+      <c r="N17" s="30"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -8620,7 +8610,7 @@
         <f aca="false">SUM(B18,C18,D18,E18,F18,G18,H18)</f>
         <v>145</v>
       </c>
-      <c r="N18" s="31"/>
+      <c r="N18" s="30"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -8641,7 +8631,7 @@
         <f aca="false">SUM(B19,C19,D19,E19,F19,G19,H19)</f>
         <v>611</v>
       </c>
-      <c r="N19" s="31"/>
+      <c r="N19" s="30"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -8662,7 +8652,7 @@
         <f aca="false">SUM(B20,C20,D20,E20,F20,G20,H20)</f>
         <v>250</v>
       </c>
-      <c r="N20" s="31"/>
+      <c r="N20" s="30"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -8683,7 +8673,7 @@
         <f aca="false">SUM(B21,C21,D21,E21,F21,G21,H21)</f>
         <v>282</v>
       </c>
-      <c r="N21" s="31"/>
+      <c r="N21" s="30"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -8702,7 +8692,7 @@
         <f aca="false">SUM(B22,C22,D22,E22,F22,G22,H22)</f>
         <v>150</v>
       </c>
-      <c r="N22" s="31"/>
+      <c r="N22" s="30"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -8721,7 +8711,7 @@
         <f aca="false">SUM(B23,C23,D23,E23,F23,G23,H23)</f>
         <v>0</v>
       </c>
-      <c r="N23" s="31"/>
+      <c r="N23" s="30"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -8744,7 +8734,7 @@
         <f aca="false">SUM(B24,C24,D24,E24,F24,G24,H24)</f>
         <v>468</v>
       </c>
-      <c r="N24" s="31"/>
+      <c r="N24" s="30"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -8765,7 +8755,7 @@
         <f aca="false">SUM(B25,C25,D25,E25,F25,G25,H25)</f>
         <v>128</v>
       </c>
-      <c r="N25" s="31"/>
+      <c r="N25" s="30"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -8784,7 +8774,7 @@
         <f aca="false">SUM(B26,C26,D26,E26,F26,G26,H26)</f>
         <v>120</v>
       </c>
-      <c r="N26" s="31"/>
+      <c r="N26" s="30"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -8807,7 +8797,7 @@
         <f aca="false">SUM(B27,C27,D27,E27,F27,G27,H27)</f>
         <v>407</v>
       </c>
-      <c r="N27" s="31"/>
+      <c r="N27" s="30"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -8826,7 +8816,7 @@
         <f aca="false">SUM(B28,C28,D28,E28,F28,G28,H28)</f>
         <v>54</v>
       </c>
-      <c r="N28" s="31"/>
+      <c r="N28" s="30"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -8845,7 +8835,7 @@
         <f aca="false">SUM(B29,C29,D29,E29,F29,G29,H29)</f>
         <v>48</v>
       </c>
-      <c r="N29" s="31"/>
+      <c r="N29" s="30"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -8868,16 +8858,16 @@
         <f aca="false">SUM(B30,C30,D30,E30,F30,G30,H30)</f>
         <v>204</v>
       </c>
-      <c r="N30" s="31"/>
+      <c r="N30" s="30"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
-      <c r="E31" s="10" t="n">
+      <c r="E31" s="0" t="n">
         <v>25</v>
       </c>
       <c r="F31" s="0"/>
@@ -8887,7 +8877,7 @@
         <f aca="false">SUM(B31,C31,D31,E31,F31,G31,H31)</f>
         <v>25</v>
       </c>
-      <c r="N31" s="31"/>
+      <c r="N31" s="30"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -8904,124 +8894,124 @@
         <f aca="false">SUM(B32,C32,D32,E32,F32,G32,H32)</f>
         <v>0</v>
       </c>
-      <c r="N32" s="31"/>
+      <c r="N32" s="30"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
-      <c r="N33" s="31"/>
+      <c r="N33" s="30"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>2458</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>3667</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>3341</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F32)</f>
         <v>1000</v>
       </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12" t="n">
+      <c r="G34" s="11"/>
+      <c r="H34" s="11" t="n">
         <f aca="false">SUM(H2:H32)</f>
         <v>4770</v>
       </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="14" t="n">
+      <c r="I34" s="12"/>
+      <c r="J34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34,H34)</f>
         <v>15236</v>
       </c>
-      <c r="N34" s="31"/>
+      <c r="N34" s="30"/>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>3667</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>200</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>700</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>350</v>
       </c>
-      <c r="H35" s="16" t="n">
+      <c r="H35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="I35" s="13"/>
-      <c r="J35" s="14" t="n">
+      <c r="I35" s="12"/>
+      <c r="J35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35,H35)</f>
         <v>6467</v>
       </c>
-      <c r="N35" s="31"/>
+      <c r="N35" s="30"/>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>-1458</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>200</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>-2641</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>-950</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>350</v>
       </c>
-      <c r="H36" s="18" t="n">
+      <c r="H36" s="17" t="n">
         <f aca="false">SUM(-H34,H35)</f>
         <v>-4270</v>
       </c>
-      <c r="J36" s="18" t="n">
+      <c r="J36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36,H36)</f>
         <v>-8769</v>
       </c>
-      <c r="N36" s="27" t="n">
+      <c r="N36" s="26" t="n">
         <f aca="false">SUM(N9:N35)</f>
         <v>1408</v>
       </c>
@@ -9071,10 +9061,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -9649,12 +9639,12 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="n">
+      <c r="B31" s="0" t="n">
         <v>22</v>
       </c>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
-      <c r="E31" s="10" t="n">
+      <c r="E31" s="0" t="n">
         <v>86</v>
       </c>
       <c r="F31" s="0"/>
@@ -9686,117 +9676,117 @@
         <f aca="false">SUM(B32,C32,D32,E32,F32,H32)</f>
         <v>106</v>
       </c>
-      <c r="N32" s="32" t="s">
-        <v>59</v>
+      <c r="N32" s="31" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>1451</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>3663</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>10</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>1781</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F32)</f>
         <v>17</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(G2:G33)</f>
         <v>729</v>
       </c>
-      <c r="H34" s="12" t="n">
+      <c r="H34" s="11" t="n">
         <f aca="false">SUM(H2:H32)</f>
         <v>5568</v>
       </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="14" t="n">
+      <c r="I34" s="12"/>
+      <c r="J34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,H34)</f>
         <v>12490</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>700</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>200</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>700</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16" t="n">
+      <c r="G35" s="15"/>
+      <c r="H35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="I35" s="13"/>
-      <c r="J35" s="14" t="n">
+      <c r="I35" s="12"/>
+      <c r="J35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,H35)</f>
         <v>3150</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>-451</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>-2963</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>190</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>-1081</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>33</v>
       </c>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18" t="n">
+      <c r="G36" s="17"/>
+      <c r="H36" s="17" t="n">
         <f aca="false">SUM(-H34,H35)</f>
         <v>-5068</v>
       </c>
-      <c r="J36" s="18" t="n">
+      <c r="J36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,H36)</f>
         <v>-9340</v>
       </c>
@@ -9846,10 +9836,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -10410,10 +10400,10 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="0"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
       <c r="I31" s="2" t="n">
@@ -10438,104 +10428,104 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>1156</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>3663</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>350</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>2215</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F32)</f>
         <v>305</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>7746.14</v>
       </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14" t="n">
+      <c r="H34" s="12"/>
+      <c r="I34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34)</f>
         <v>15435.14</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>3663</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>200</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>2585</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14" t="n">
+      <c r="H35" s="12"/>
+      <c r="I35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35)</f>
         <v>7998</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>-156</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>-150</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>-1715</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>-255</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>-5161.14</v>
       </c>
-      <c r="I36" s="18" t="n">
+      <c r="I36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36)</f>
         <v>-7437.14</v>
       </c>
@@ -10585,10 +10575,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -10818,9 +10808,7 @@
       <c r="B14" s="0"/>
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
-      <c r="E14" s="0" t="s">
-        <v>14</v>
-      </c>
+      <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
       <c r="I14" s="2" t="n">
@@ -11108,10 +11096,10 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="0"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0" t="n">
         <v>105</v>
@@ -11142,104 +11130,104 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>0</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>1000</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>1732</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F32)</f>
         <v>1338</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>5305</v>
       </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14" t="n">
+      <c r="H34" s="12"/>
+      <c r="I34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34)</f>
         <v>9375</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>700</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>200</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>1500</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14" t="n">
+      <c r="H35" s="12"/>
+      <c r="I35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35)</f>
         <v>4450</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>1000</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>-300</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>200</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>-732</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>-1288</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>-3805</v>
       </c>
-      <c r="I36" s="18" t="n">
+      <c r="I36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36)</f>
         <v>-4925</v>
       </c>
@@ -11291,10 +11279,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -11834,10 +11822,10 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
-      <c r="E31" s="10" t="n">
+      <c r="E31" s="0" t="n">
         <v>135</v>
       </c>
       <c r="F31" s="0"/>
@@ -11864,71 +11852,71 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>794</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>1500</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>514</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>1297</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F32)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>762</v>
       </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14" t="n">
+      <c r="H34" s="12"/>
+      <c r="I34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34)</f>
         <v>4867</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>750</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14" t="n">
+      <c r="H35" s="12"/>
+      <c r="I35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35)</f>
         <v>3800</v>
       </c>
@@ -11937,34 +11925,34 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>206</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>-500</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>236</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,1000)</f>
         <v>-297</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>50</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>-262</v>
       </c>
-      <c r="I36" s="18" t="n">
+      <c r="I36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36)</f>
         <v>-567</v>
       </c>
@@ -12018,10 +12006,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -12032,7 +12020,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -12058,7 +12046,7 @@
       <c r="G2" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="I2" s="14" t="n">
+      <c r="I2" s="13" t="n">
         <f aca="false">SUM(B2,C2,D2,E2,F2,G2)</f>
         <v>652</v>
       </c>
@@ -12085,7 +12073,7 @@
       <c r="G3" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="I3" s="14" t="n">
+      <c r="I3" s="13" t="n">
         <f aca="false">SUM(B3,C3,D3,E3,F3,G3)</f>
         <v>110</v>
       </c>
@@ -12112,7 +12100,7 @@
       <c r="G4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I4" s="14" t="n">
+      <c r="I4" s="13" t="n">
         <f aca="false">SUM(B4,C4,D4,E4,F4,G4)</f>
         <v>74</v>
       </c>
@@ -12139,7 +12127,7 @@
       <c r="G5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="14" t="n">
+      <c r="I5" s="13" t="n">
         <f aca="false">SUM(B5,C5,D5,E5,F5,G5)</f>
         <v>20</v>
       </c>
@@ -12166,7 +12154,7 @@
       <c r="G6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="14" t="n">
+      <c r="I6" s="13" t="n">
         <f aca="false">SUM(B6,C6,D6,E6,F6,G6)</f>
         <v>48</v>
       </c>
@@ -12193,12 +12181,12 @@
       <c r="G7" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="I7" s="14" t="n">
+      <c r="I7" s="13" t="n">
         <f aca="false">SUM(B7,C7,D7,E7,F7,G7)</f>
         <v>81</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12223,7 +12211,7 @@
       <c r="G8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="14" t="n">
+      <c r="I8" s="13" t="n">
         <f aca="false">SUM(B8,C8,D8,E8,F8,G8)</f>
         <v>69</v>
       </c>
@@ -12253,7 +12241,7 @@
       <c r="G9" s="0" t="n">
         <v>344</v>
       </c>
-      <c r="I9" s="14" t="n">
+      <c r="I9" s="13" t="n">
         <f aca="false">SUM(B9,C9,D9,E9,F9,G9)</f>
         <v>712</v>
       </c>
@@ -12283,7 +12271,7 @@
       <c r="G10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="14" t="n">
+      <c r="I10" s="13" t="n">
         <f aca="false">SUM(B10,C10,D10,E10,F10,G10)</f>
         <v>70</v>
       </c>
@@ -12310,7 +12298,7 @@
       <c r="G11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="14" t="n">
+      <c r="I11" s="13" t="n">
         <f aca="false">SUM(B11,C11,D11,E11,F11,G11)</f>
         <v>69</v>
       </c>
@@ -12337,7 +12325,7 @@
       <c r="G12" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="I12" s="14" t="n">
+      <c r="I12" s="13" t="n">
         <f aca="false">SUM(B12,C12,D12,E12,F12,G12)</f>
         <v>150</v>
       </c>
@@ -12367,7 +12355,7 @@
       <c r="G13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="14" t="n">
+      <c r="I13" s="13" t="n">
         <f aca="false">SUM(B13,C13,D13,E13,F13,G13)</f>
         <v>0</v>
       </c>
@@ -12397,7 +12385,7 @@
       <c r="G14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="14" t="n">
+      <c r="I14" s="13" t="n">
         <f aca="false">SUM(B14,C14,D14,E14,F14,G14)</f>
         <v>78</v>
       </c>
@@ -12427,7 +12415,7 @@
       <c r="G15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="14" t="n">
+      <c r="I15" s="13" t="n">
         <f aca="false">SUM(B15,C15,D15,E15,F15,G15)</f>
         <v>526</v>
       </c>
@@ -12457,7 +12445,7 @@
       <c r="G16" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="14" t="n">
+      <c r="I16" s="13" t="n">
         <f aca="false">SUM(B16,C16,D16,E16,F16,G16)</f>
         <v>108</v>
       </c>
@@ -12484,7 +12472,7 @@
       <c r="G17" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="14" t="n">
+      <c r="I17" s="13" t="n">
         <f aca="false">SUM(B17,C17,D17,E17,F17,G17)</f>
         <v>61</v>
       </c>
@@ -12511,7 +12499,7 @@
       <c r="G18" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="14" t="n">
+      <c r="I18" s="13" t="n">
         <f aca="false">SUM(B18,C18,D18,E18,F18,G18)</f>
         <v>167</v>
       </c>
@@ -12538,7 +12526,7 @@
       <c r="G19" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="14" t="n">
+      <c r="I19" s="13" t="n">
         <f aca="false">SUM(B19,C19,D19,E19,F19,G19)</f>
         <v>40</v>
       </c>
@@ -12565,7 +12553,7 @@
       <c r="G20" s="0" t="n">
         <v>135</v>
       </c>
-      <c r="I20" s="14" t="n">
+      <c r="I20" s="13" t="n">
         <f aca="false">SUM(B20,C20,D20,E20,F20,G20)</f>
         <v>135</v>
       </c>
@@ -12592,7 +12580,7 @@
       <c r="G21" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="14" t="n">
+      <c r="I21" s="13" t="n">
         <f aca="false">SUM(B21,C21,D21,E21,F21,G21)</f>
         <v>173</v>
       </c>
@@ -12619,7 +12607,7 @@
       <c r="G22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I22" s="14" t="n">
+      <c r="I22" s="13" t="n">
         <f aca="false">SUM(B22,C22,D22,E22,F22,G22)</f>
         <v>116</v>
       </c>
@@ -12646,7 +12634,7 @@
       <c r="G23" s="0" t="n">
         <v>400</v>
       </c>
-      <c r="I23" s="14" t="n">
+      <c r="I23" s="13" t="n">
         <f aca="false">SUM(B23,C23,D23,E23,F23,G23)</f>
         <v>505</v>
       </c>
@@ -12673,7 +12661,7 @@
       <c r="G24" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I24" s="14" t="n">
+      <c r="I24" s="13" t="n">
         <f aca="false">SUM(B24,C24,D24,E24,F24,G24)</f>
         <v>35</v>
       </c>
@@ -12700,7 +12688,7 @@
       <c r="G25" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I25" s="14" t="n">
+      <c r="I25" s="13" t="n">
         <f aca="false">SUM(B25,C25,D25,E25,F25,G25)</f>
         <v>70</v>
       </c>
@@ -12727,7 +12715,7 @@
       <c r="G26" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I26" s="14" t="n">
+      <c r="I26" s="13" t="n">
         <f aca="false">SUM(B26,C26,D26,E26,F26,G26)</f>
         <v>20</v>
       </c>
@@ -12754,7 +12742,7 @@
       <c r="G27" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I27" s="14" t="n">
+      <c r="I27" s="13" t="n">
         <f aca="false">SUM(B27,C27,D27,E27,F27,G27)</f>
         <v>60</v>
       </c>
@@ -12781,7 +12769,7 @@
       <c r="G28" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I28" s="14" t="n">
+      <c r="I28" s="13" t="n">
         <f aca="false">SUM(B28,C28,D28,E28,F28,G28)</f>
         <v>63</v>
       </c>
@@ -12808,7 +12796,7 @@
       <c r="G29" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I29" s="14" t="n">
+      <c r="I29" s="13" t="n">
         <f aca="false">SUM(B29,C29,D29,E29,F29,G29)</f>
         <v>20</v>
       </c>
@@ -12835,7 +12823,7 @@
       <c r="G30" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I30" s="14" t="n">
+      <c r="I30" s="13" t="n">
         <f aca="false">SUM(B30,C30,D30,E30,F30,G30)</f>
         <v>171</v>
       </c>
@@ -12844,7 +12832,7 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="n">
+      <c r="B31" s="0" t="n">
         <v>78</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -12853,7 +12841,7 @@
       <c r="D31" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E31" s="10" t="n">
+      <c r="E31" s="0" t="n">
         <v>28</v>
       </c>
       <c r="F31" s="0" t="n">
@@ -12862,7 +12850,7 @@
       <c r="G31" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I31" s="14" t="n">
+      <c r="I31" s="13" t="n">
         <f aca="false">SUM(B31,C31,D31,E31,F31,G31)</f>
         <v>106</v>
       </c>
@@ -12892,51 +12880,51 @@
       <c r="G32" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I32" s="14" t="n">
+      <c r="I32" s="13" t="n">
         <f aca="false">SUM(B32,C32,D32,E32,F32,G32)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
-      <c r="I33" s="13"/>
+      <c r="I33" s="12"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>1365</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>1000</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>859</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F32)</f>
         <v>10</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>1275</v>
       </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14" t="n">
+      <c r="H34" s="12"/>
+      <c r="I34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34)</f>
         <v>4509</v>
       </c>
@@ -12946,34 +12934,34 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="18" t="n">
+      <c r="A35" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="17" t="n">
         <f aca="false">SUM(-B34,1500)</f>
         <v>135</v>
       </c>
-      <c r="C35" s="18" t="n">
+      <c r="C35" s="17" t="n">
         <f aca="false">SUM(-C34,1000)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="18" t="n">
+      <c r="D35" s="17" t="n">
         <f aca="false">SUM(-D34,200)</f>
         <v>200</v>
       </c>
-      <c r="E35" s="18" t="n">
+      <c r="E35" s="17" t="n">
         <f aca="false">SUM(-E34,500)</f>
         <v>-359</v>
       </c>
-      <c r="F35" s="18" t="n">
+      <c r="F35" s="17" t="n">
         <f aca="false">SUM(-F34,100)</f>
         <v>90</v>
       </c>
-      <c r="G35" s="18" t="n">
+      <c r="G35" s="17" t="n">
         <f aca="false">SUM(-G34,1400)</f>
         <v>125</v>
       </c>
-      <c r="I35" s="18" t="n">
+      <c r="I35" s="17" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35)</f>
         <v>191</v>
       </c>
@@ -13019,16 +13007,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -13496,287 +13484,287 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="33" t="n">
+      <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="33" t="n">
+      <c r="B22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="33" t="n">
+      <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="33" t="n">
+      <c r="B23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="0" t="n">
         <v>744</v>
       </c>
-      <c r="E23" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" s="33" t="n">
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G23" s="33" t="n">
+      <c r="G23" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="33" t="n">
+      <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="33" t="n">
+      <c r="B24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="33" t="n">
+      <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="33" t="n">
+      <c r="B25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F25" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="33" t="n">
+      <c r="F25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="33" t="n">
+      <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="33" t="n">
+      <c r="B26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="F26" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="33" t="n">
+      <c r="F26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="0" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="33" t="n">
+      <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="33" t="n">
+      <c r="B27" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="C27" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" s="33" t="n">
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="0" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="33" t="n">
+      <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C28" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="33" t="n">
+      <c r="B28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="F28" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" s="33" t="n">
+      <c r="F28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="33" t="n">
+      <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C29" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="33" t="n">
+      <c r="B29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="0" t="n">
         <v>138</v>
       </c>
-      <c r="F29" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" s="33" t="n">
+      <c r="F29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="0" t="n">
         <v>227</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="33" t="n">
+      <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="33" t="n">
+      <c r="B30" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C30" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" s="33" t="n">
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="33" t="n">
+      <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="33" t="n">
+      <c r="B31" s="0" t="n">
         <v>69</v>
       </c>
-      <c r="C31" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" s="33" t="n">
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="F31" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" s="33" t="n">
+      <c r="F31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="33" t="n">
+      <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="33" t="n">
+      <c r="B32" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="C32" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="33" t="n">
+      <c r="C32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
         <v>99</v>
       </c>
-      <c r="F32" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" s="33" t="n">
+      <c r="F32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="0" t="n">
         <v>70</v>
       </c>
     </row>
-    <row r="33" s="34" customFormat="true" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="21" t="n">
+    <row r="33" s="32" customFormat="true" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="20" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>1905</v>
       </c>
-      <c r="C33" s="21" t="n">
+      <c r="C33" s="20" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>1300</v>
       </c>
-      <c r="D33" s="21" t="n">
+      <c r="D33" s="20" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>904</v>
       </c>
-      <c r="E33" s="21" t="n">
+      <c r="E33" s="20" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>1047</v>
       </c>
-      <c r="F33" s="21" t="n">
+      <c r="F33" s="20" t="n">
         <f aca="false">SUM(F2:F32)</f>
         <v>16</v>
       </c>
-      <c r="G33" s="21" t="n">
+      <c r="G33" s="20" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>1282</v>
       </c>
-      <c r="I33" s="34" t="n">
+      <c r="I33" s="32" t="n">
         <f aca="false">SUM(B33,C33,D33,E33,F33,G33)</f>
         <v>6454</v>
       </c>
@@ -14287,9 +14275,9 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="0"/>
-      <c r="D31" s="10"/>
+      <c r="D31" s="0"/>
       <c r="E31" s="0"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
@@ -14315,104 +14303,104 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
-      <c r="D33" s="10"/>
+      <c r="D33" s="0"/>
       <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
+        <f aca="false">SUM(B2:B32)</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="11" t="n">
+        <f aca="false">SUM(C2:C32)</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="11" t="n">
+        <f aca="false">SUM(D2:D32)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="11" t="n">
+        <f aca="false">SUM(E2:E32)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="11" t="n">
+        <f aca="false">SUM(F2:F33)</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="11" t="n">
+        <f aca="false">SUM(G2:G32)</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="13" t="n">
+        <f aca="false">SUM(B34,C34,D34,E34,F34,G34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="12" t="n">
-        <f aca="false">SUM(B2:B32)</f>
-        <v>0</v>
-      </c>
-      <c r="C34" s="12" t="n">
-        <f aca="false">SUM(C2:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="12" t="n">
-        <f aca="false">SUM(D2:D32)</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="12" t="n">
-        <f aca="false">SUM(E2:E32)</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="12" t="n">
-        <f aca="false">SUM(F2:F33)</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="12" t="n">
-        <f aca="false">SUM(G2:G32)</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14" t="n">
-        <f aca="false">SUM(B34,C34,D34,E34,F34,G34)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="B35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>4000</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>700</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>350</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14" t="n">
+      <c r="H35" s="12"/>
+      <c r="I35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35)</f>
         <v>6600</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>1000</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>4000</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>700</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>50</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>350</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>500</v>
       </c>
-      <c r="I36" s="18" t="n">
+      <c r="I36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36)</f>
         <v>6600</v>
       </c>
@@ -14516,17 +14504,17 @@
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="20" t="s">
+      <c r="O2" s="18"/>
+      <c r="P2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20" t="s">
+      <c r="S2" s="19"/>
+      <c r="U2" s="20" t="s">
         <v>27</v>
-      </c>
-      <c r="S2" s="20"/>
-      <c r="U2" s="21" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14556,18 +14544,18 @@
         <v>160</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N3" s="6" t="n">
         <v>2000</v>
       </c>
-      <c r="O3" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
+      <c r="O3" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
       <c r="U3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14595,16 +14583,16 @@
         <v>4000</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N4" s="6" t="n">
         <v>5000</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
       <c r="U4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14630,16 +14618,16 @@
         <v>15800</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N5" s="6" t="n">
         <v>5000</v>
       </c>
-      <c r="O5" s="19"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
       <c r="U5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14668,13 +14656,13 @@
       <c r="L6" s="5"/>
       <c r="M6" s="4"/>
       <c r="N6" s="6"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="18" t="n">
+      <c r="O6" s="18"/>
+      <c r="P6" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
       <c r="U6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14695,19 +14683,17 @@
         <f aca="false">SUM(B7,C7,D7,E7,F7,G7)</f>
         <v>662</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="K7" s="4"/>
       <c r="L7" s="5"/>
       <c r="M7" s="4"/>
       <c r="N7" s="6"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18" t="n">
+      <c r="O7" s="18"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="S7" s="18"/>
+      <c r="S7" s="17"/>
       <c r="U7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14740,11 +14726,11 @@
         <f aca="false">SUM(N2:N7)</f>
         <v>12000</v>
       </c>
-      <c r="O8" s="19"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
       <c r="U8" s="9" t="n">
         <v>270</v>
       </c>
@@ -14769,10 +14755,10 @@
         <f aca="false">SUM(B9,C9,D9,E9,F9,G9)</f>
         <v>235</v>
       </c>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
       <c r="U9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14793,10 +14779,10 @@
         <f aca="false">SUM(B10,C10,D10,E10,F10,G10)</f>
         <v>595</v>
       </c>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
       <c r="U10" s="9" t="n">
         <v>274</v>
       </c>
@@ -14817,10 +14803,10 @@
         <f aca="false">SUM(B11,C11,D11,E11,F11,G11)</f>
         <v>344</v>
       </c>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
       <c r="U11" s="9" t="n">
         <v>344</v>
       </c>
@@ -14847,10 +14833,10 @@
         <f aca="false">SUM(B12,C12,D12,E12,F12,G12)</f>
         <v>2015</v>
       </c>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
       <c r="U12" s="9" t="n">
         <v>1423</v>
       </c>
@@ -14871,10 +14857,10 @@
         <f aca="false">SUM(B13,C13,D13,E13,F13,G13)</f>
         <v>110</v>
       </c>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
       <c r="U13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14897,10 +14883,10 @@
         <f aca="false">SUM(B14,C14,D14,E14,F14,G14)</f>
         <v>836</v>
       </c>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
       <c r="U14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14919,10 +14905,10 @@
         <f aca="false">SUM(B15,C15,D15,E15,F15,G15)</f>
         <v>125</v>
       </c>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
       <c r="U15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14948,15 +14934,15 @@
         <v>959</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L16" s="7"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="19"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="18"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
       <c r="U16" s="9" t="n">
         <v>438</v>
       </c>
@@ -14982,17 +14968,17 @@
         <v>4209</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L17" s="9" t="n">
         <v>6000</v>
       </c>
-      <c r="M17" s="22"/>
-      <c r="N17" s="19"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="18"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
       <c r="U17" s="9" t="n">
         <v>290</v>
       </c>
@@ -15014,19 +15000,19 @@
         <v>1294</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L18" s="9" t="n">
         <v>700</v>
       </c>
-      <c r="M18" s="22" t="n">
+      <c r="M18" s="21" t="n">
         <v>600</v>
       </c>
-      <c r="N18" s="19"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
       <c r="U18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15048,19 +15034,19 @@
         <v>767</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L19" s="9" t="n">
         <v>300</v>
       </c>
-      <c r="M19" s="22" t="n">
+      <c r="M19" s="21" t="n">
         <v>50</v>
       </c>
-      <c r="N19" s="19"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
       <c r="U19" s="9" t="n">
         <v>637</v>
       </c>
@@ -15087,12 +15073,12 @@
       <c r="L20" s="9" t="n">
         <v>500</v>
       </c>
-      <c r="M20" s="22"/>
-      <c r="N20" s="19"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="18"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
       <c r="U20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15117,12 +15103,12 @@
       </c>
       <c r="K21" s="8"/>
       <c r="L21" s="9"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="19"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="18"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
       <c r="U21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15142,17 +15128,17 @@
         <v>230</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L22" s="9" t="n">
         <v>600</v>
       </c>
-      <c r="M22" s="22"/>
-      <c r="N22" s="19"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="18"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
       <c r="U22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15172,17 +15158,17 @@
         <v>40</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L23" s="9" t="n">
         <v>1000</v>
       </c>
-      <c r="M23" s="22"/>
-      <c r="N23" s="19"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="18"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
       <c r="U23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15202,19 +15188,19 @@
         <v>42</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L24" s="9" t="n">
         <v>700</v>
       </c>
-      <c r="M24" s="22" t="n">
+      <c r="M24" s="21" t="n">
         <v>732</v>
       </c>
-      <c r="N24" s="19"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
       <c r="U24" s="9" t="n">
         <v>42</v>
       </c>
@@ -15236,19 +15222,19 @@
         <v>300</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L25" s="9" t="n">
         <v>1500</v>
       </c>
-      <c r="M25" s="22" t="n">
+      <c r="M25" s="21" t="n">
         <v>1423</v>
       </c>
-      <c r="N25" s="19"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
       <c r="U25" s="9" t="n">
         <v>300</v>
       </c>
@@ -15271,12 +15257,12 @@
       </c>
       <c r="K26" s="8"/>
       <c r="L26" s="9"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="19"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="18"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
       <c r="U26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15299,12 +15285,12 @@
       </c>
       <c r="K27" s="8"/>
       <c r="L27" s="9"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="19"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="18"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
       <c r="U27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15325,12 +15311,12 @@
       </c>
       <c r="K28" s="8"/>
       <c r="L28" s="9"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="19"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="18"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
       <c r="U28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15349,12 +15335,12 @@
       </c>
       <c r="K29" s="8"/>
       <c r="L29" s="9"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="19"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="18"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="18"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
       <c r="U29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15373,21 +15359,21 @@
       </c>
       <c r="K30" s="8"/>
       <c r="L30" s="9"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="19"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="18"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
       <c r="U30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="0"/>
-      <c r="D31" s="10"/>
+      <c r="D31" s="0"/>
       <c r="E31" s="0"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
@@ -15400,15 +15386,15 @@
         <f aca="false">SUM(L17:L30)</f>
         <v>11300</v>
       </c>
-      <c r="M31" s="22" t="n">
+      <c r="M31" s="21" t="n">
         <f aca="false">SUM(M17:M30)</f>
         <v>2805</v>
       </c>
-      <c r="N31" s="19"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
       <c r="U31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15425,127 +15411,127 @@
         <f aca="false">SUM(B32,C32,D32,E32,F32,G32)</f>
         <v>0</v>
       </c>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
       <c r="U32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
-      <c r="D33" s="10"/>
+      <c r="D33" s="0"/>
       <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="24" t="n">
+      <c r="A34" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="23" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>3208</v>
       </c>
-      <c r="C34" s="24" t="n">
+      <c r="C34" s="23" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>3363</v>
       </c>
-      <c r="D34" s="24" t="n">
+      <c r="D34" s="23" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>1477</v>
       </c>
-      <c r="E34" s="24" t="n">
+      <c r="E34" s="23" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>506</v>
       </c>
-      <c r="F34" s="24" t="n">
+      <c r="F34" s="23" t="n">
         <f aca="false">SUM(F2:F33)</f>
         <v>524</v>
       </c>
-      <c r="G34" s="24" t="n">
+      <c r="G34" s="23" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>8829</v>
       </c>
-      <c r="H34" s="25"/>
-      <c r="I34" s="26" t="n">
+      <c r="H34" s="24"/>
+      <c r="I34" s="25" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34)</f>
         <v>17907</v>
       </c>
-      <c r="P34" s="27" t="n">
+      <c r="P34" s="26" t="n">
         <f aca="false">SUM(P3:P33)</f>
         <v>10</v>
       </c>
-      <c r="Q34" s="27"/>
-      <c r="R34" s="27" t="n">
+      <c r="Q34" s="26"/>
+      <c r="R34" s="26" t="n">
         <f aca="false">SUM(R3:R32)</f>
         <v>15</v>
       </c>
-      <c r="S34" s="27"/>
+      <c r="S34" s="26"/>
       <c r="U34" s="0" t="n">
         <f aca="false">SUM(U3,U4,U5,U6,U7,U8,U9,U10,U11,U12,U13,U14,U15,U16,U17,U18,U19,U20,U21,U22,U23,U24,U25,U26,U27,U28,U29,U30,U31,U32)</f>
         <v>4018</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="29" t="n">
+      <c r="A35" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="28" t="n">
         <v>3000</v>
       </c>
-      <c r="C35" s="29" t="n">
+      <c r="C35" s="28" t="n">
         <v>3800</v>
       </c>
-      <c r="D35" s="29" t="n">
+      <c r="D35" s="28" t="n">
         <v>1500</v>
       </c>
-      <c r="E35" s="29" t="n">
+      <c r="E35" s="28" t="n">
         <v>1050</v>
       </c>
-      <c r="F35" s="29" t="n">
+      <c r="F35" s="28" t="n">
         <v>400</v>
       </c>
-      <c r="G35" s="29" t="n">
+      <c r="G35" s="28" t="n">
         <f aca="false">SUM(L17:L30)</f>
         <v>11300</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="26" t="n">
+      <c r="H35" s="24"/>
+      <c r="I35" s="25" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35)</f>
         <v>21050</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>-208</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>437</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>23</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>544</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>-124</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>2471</v>
       </c>
-      <c r="I36" s="18" t="n">
+      <c r="I36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36)</f>
         <v>3143</v>
       </c>
@@ -15671,9 +15657,6 @@
         <f aca="false">SUM(B4,C4,D4,E4,F4,G4)</f>
         <v>90</v>
       </c>
-      <c r="K4" s="0" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -15814,7 +15797,7 @@
         <v>40</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M11" s="0" t="n">
         <v>1000</v>
@@ -15841,7 +15824,7 @@
         <v>645</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M12" s="0" t="n">
         <v>500</v>
@@ -15866,7 +15849,7 @@
         <v>122</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>300</v>
@@ -15889,7 +15872,7 @@
         <v>50</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M14" s="0" t="n">
         <v>6000</v>
@@ -16038,17 +16021,17 @@
         <f aca="false">SUM(B22,C22,D22,E22,F22,G22)</f>
         <v>25</v>
       </c>
-      <c r="O22" s="30" t="s">
+      <c r="O22" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="P22" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="P22" s="30" t="s">
+      <c r="Q22" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="Q22" s="0" t="s">
+      <c r="R22" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="R22" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16067,8 +16050,8 @@
         <f aca="false">SUM(B23,C23,D23,E23,F23,G23)</f>
         <v>20</v>
       </c>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -16086,10 +16069,10 @@
         <f aca="false">SUM(B24,C24,D24,E24,F24,G24)</f>
         <v>82</v>
       </c>
-      <c r="O24" s="30" t="n">
+      <c r="O24" s="29" t="n">
         <v>5</v>
       </c>
-      <c r="P24" s="30" t="n">
+      <c r="P24" s="29" t="n">
         <v>10</v>
       </c>
     </row>
@@ -16109,10 +16092,10 @@
         <f aca="false">SUM(B25,C25,D25,E25,F25,G25)</f>
         <v>125</v>
       </c>
-      <c r="O25" s="30" t="n">
+      <c r="O25" s="29" t="n">
         <v>25</v>
       </c>
-      <c r="P25" s="30" t="n">
+      <c r="P25" s="29" t="n">
         <v>10</v>
       </c>
     </row>
@@ -16134,8 +16117,8 @@
         <f aca="false">SUM(B26,C26,D26,E26,F26,G26)</f>
         <v>205</v>
       </c>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -16157,8 +16140,8 @@
         <f aca="false">SUM(B27,C27,D27,E27,F27,G27)</f>
         <v>660</v>
       </c>
-      <c r="O27" s="30"/>
-      <c r="P27" s="30"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -16178,8 +16161,8 @@
         <f aca="false">SUM(B28,C28,D28,E28,F28,G28)</f>
         <v>90</v>
       </c>
-      <c r="O28" s="30"/>
-      <c r="P28" s="30"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -16197,10 +16180,10 @@
         <f aca="false">SUM(B29,C29,D29,E29,F29,G29)</f>
         <v>65</v>
       </c>
-      <c r="O29" s="30" t="n">
+      <c r="O29" s="29" t="n">
         <v>10</v>
       </c>
-      <c r="P29" s="30" t="n">
+      <c r="P29" s="29" t="n">
         <v>10</v>
       </c>
     </row>
@@ -16222,8 +16205,8 @@
         <f aca="false">SUM(B30,C30,D30,E30,F30,G30)</f>
         <v>385</v>
       </c>
-      <c r="O30" s="30"/>
-      <c r="P30" s="30" t="n">
+      <c r="O30" s="29"/>
+      <c r="P30" s="29" t="n">
         <v>110</v>
       </c>
       <c r="Q30" s="0" t="n">
@@ -16234,9 +16217,9 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="0"/>
-      <c r="D31" s="10" t="n">
+      <c r="D31" s="0" t="n">
         <v>60</v>
       </c>
       <c r="E31" s="0"/>
@@ -16246,8 +16229,8 @@
         <f aca="false">SUM(B31,C31,D31,E31,F31,G31)</f>
         <v>60</v>
       </c>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30" t="n">
+      <c r="O31" s="29"/>
+      <c r="P31" s="29" t="n">
         <v>10</v>
       </c>
       <c r="R31" s="0" t="n">
@@ -16268,58 +16251,58 @@
         <f aca="false">SUM(B32,C32,D32,E32,F32,G32)</f>
         <v>0</v>
       </c>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
-      <c r="D33" s="10"/>
+      <c r="D33" s="0"/>
       <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="29"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>848</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>4008</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>1919</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>790</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F33)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>7700</v>
       </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14" t="n">
+      <c r="H34" s="12"/>
+      <c r="I34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34)</f>
         <v>15265</v>
       </c>
-      <c r="O34" s="30" t="n">
+      <c r="O34" s="29" t="n">
         <f aca="false">SUM(O24:O33)</f>
         <v>40</v>
       </c>
-      <c r="P34" s="30" t="n">
+      <c r="P34" s="29" t="n">
         <f aca="false">SUM(P23:P33)</f>
         <v>150</v>
       </c>
@@ -16333,69 +16316,69 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1500</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>3800</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>1050</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>350</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>8300</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14" t="n">
+      <c r="H35" s="12"/>
+      <c r="I35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35)</f>
         <v>16000</v>
       </c>
-      <c r="O35" s="30"/>
-      <c r="P35" s="30"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="29"/>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>652</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>-208</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>-919</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>260</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>350</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>600</v>
       </c>
-      <c r="I36" s="18" t="n">
+      <c r="I36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36)</f>
         <v>735</v>
       </c>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -17002,9 +16985,9 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="0"/>
-      <c r="D31" s="10" t="n">
+      <c r="D31" s="0" t="n">
         <v>40</v>
       </c>
       <c r="E31" s="0"/>
@@ -17034,104 +17017,104 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
-      <c r="D33" s="10"/>
+      <c r="D33" s="0"/>
       <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>1653</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>3667</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>1978</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>162</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F33)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>23360</v>
       </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14" t="n">
+      <c r="H34" s="12"/>
+      <c r="I34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34)</f>
         <v>30820</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>4000</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>700</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>350</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14" t="n">
+      <c r="H35" s="12"/>
+      <c r="I35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35)</f>
         <v>6600</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>-653</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>333</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>-1278</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>-112</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>350</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>-22860</v>
       </c>
-      <c r="I36" s="18" t="n">
+      <c r="I36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36)</f>
         <v>-24220</v>
       </c>
@@ -17781,11 +17764,11 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="n">
+      <c r="B31" s="0" t="n">
         <v>374</v>
       </c>
       <c r="C31" s="0"/>
-      <c r="D31" s="10"/>
+      <c r="D31" s="0"/>
       <c r="E31" s="0"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
@@ -17811,104 +17794,104 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
-      <c r="D33" s="10"/>
+      <c r="D33" s="0"/>
       <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>2865</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>6289</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>2319</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>679</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F33)</f>
         <v>480</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>4425</v>
       </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14" t="n">
+      <c r="H34" s="12"/>
+      <c r="I34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34)</f>
         <v>17057</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>700</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>350</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14" t="n">
+      <c r="H35" s="12"/>
+      <c r="I35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35)</f>
         <v>3600</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>-1865</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>-5289</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>-1619</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>-629</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>-130</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>-3925</v>
       </c>
-      <c r="I36" s="18" t="n">
+      <c r="I36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36)</f>
         <v>-13457</v>
       </c>
@@ -17960,10 +17943,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -17981,7 +17964,7 @@
         <v>7</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18086,7 +18069,7 @@
         <v>10119</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18551,10 +18534,10 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
-      <c r="E31" s="10" t="n">
+      <c r="E31" s="0" t="n">
         <v>170</v>
       </c>
       <c r="F31" s="0"/>
@@ -18585,79 +18568,79 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>1206</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>700</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>40</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>2009</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F32)</f>
         <v>161</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(A34:F34)</f>
         <v>4116</v>
       </c>
-      <c r="H34" s="12" t="n">
+      <c r="H34" s="11" t="n">
         <f aca="false">SUM(H2:H32)</f>
         <v>13383</v>
       </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="14" t="n">
+      <c r="I34" s="12"/>
+      <c r="J34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34,H34)</f>
         <v>21615</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>200</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>700</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>350</v>
       </c>
-      <c r="H35" s="16" t="n">
+      <c r="H35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="I35" s="13"/>
-      <c r="J35" s="14" t="n">
+      <c r="I35" s="12"/>
+      <c r="J35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35,H35)</f>
         <v>3800</v>
       </c>
@@ -18666,38 +18649,38 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>-206</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>300</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>160</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>-1309</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>-111</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>-3766</v>
       </c>
-      <c r="H36" s="18" t="n">
+      <c r="H36" s="17" t="n">
         <f aca="false">SUM(-H34,H35)</f>
         <v>-12883</v>
       </c>
-      <c r="J36" s="18" t="n">
+      <c r="J36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36,H36)</f>
         <v>-17815</v>
       </c>
@@ -18753,10 +18736,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -19158,7 +19141,7 @@
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F22" s="0"/>
       <c r="G22" s="0"/>
@@ -19310,10 +19293,10 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="0"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
       <c r="H31" s="0"/>
@@ -19340,113 +19323,113 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>1326</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>1000</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>1924</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F32)</f>
         <v>422</v>
       </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12" t="n">
+      <c r="G34" s="11"/>
+      <c r="H34" s="11" t="n">
         <f aca="false">SUM(H2:H32)</f>
         <v>5151</v>
       </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="14" t="n">
+      <c r="I34" s="12"/>
+      <c r="J34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34,H34)</f>
         <v>9823</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>200</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>700</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>350</v>
       </c>
-      <c r="H35" s="16" t="n">
+      <c r="H35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="I35" s="13"/>
-      <c r="J35" s="14" t="n">
+      <c r="I35" s="12"/>
+      <c r="J35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35,H35)</f>
         <v>3800</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>-326</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>200</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>-1224</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>-372</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>350</v>
       </c>
-      <c r="H36" s="18" t="n">
+      <c r="H36" s="17" t="n">
         <f aca="false">SUM(-H34,H35)</f>
         <v>-4651</v>
       </c>
-      <c r="J36" s="18" t="n">
+      <c r="J36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36,H36)</f>
         <v>-6023</v>
       </c>
@@ -19498,10 +19481,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -19781,7 +19764,7 @@
         <v>68</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19802,7 +19785,7 @@
         <v>255</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19987,7 +19970,7 @@
         <v>2944</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20086,10 +20069,10 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
-      <c r="E31" s="10" t="n">
+      <c r="E31" s="0" t="n">
         <v>25</v>
       </c>
       <c r="F31" s="0"/>
@@ -20120,116 +20103,116 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>1269</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>1000</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>1691</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F32)</f>
         <v>1000</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(A34:F34)</f>
         <v>4960</v>
       </c>
-      <c r="H34" s="12" t="n">
+      <c r="H34" s="11" t="n">
         <f aca="false">SUM(H2:H32)</f>
         <v>5679</v>
       </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="14" t="n">
+      <c r="I34" s="12"/>
+      <c r="J34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34,H34)</f>
         <v>15599</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>200</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>700</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>350</v>
       </c>
-      <c r="H35" s="16" t="n">
+      <c r="H35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="I35" s="13"/>
-      <c r="J35" s="14" t="n">
+      <c r="I35" s="12"/>
+      <c r="J35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35,H35)</f>
         <v>3800</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>-269</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>200</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>-991</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>-950</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>-4610</v>
       </c>
-      <c r="H36" s="18" t="n">
+      <c r="H36" s="17" t="n">
         <f aca="false">SUM(-H34,H35)</f>
         <v>-5179</v>
       </c>
-      <c r="J36" s="18" t="n">
+      <c r="J36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36,H36)</f>
         <v>-11799</v>
       </c>
@@ -20284,7 +20267,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -20324,10 +20307,10 @@
         <v>557</v>
       </c>
       <c r="M2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20358,7 +20341,7 @@
         <v>3000</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20379,10 +20362,10 @@
         <v>18</v>
       </c>
       <c r="N4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20406,7 +20389,7 @@
         <v>370</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20432,7 +20415,7 @@
         <v>500</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20668,7 +20651,7 @@
         <v>200</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20770,7 +20753,7 @@
         <v>100</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20911,12 +20894,12 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="n">
+      <c r="B31" s="0" t="n">
         <v>300</v>
       </c>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="0"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
       <c r="H31" s="0"/>
@@ -20947,116 +20930,116 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="0"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="n">
+      <c r="A34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="11" t="n">
         <f aca="false">SUM(B2:B32)</f>
         <v>1710</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="11" t="n">
         <f aca="false">SUM(C2:C32)</f>
         <v>7973</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <f aca="false">SUM(D2:D32)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <f aca="false">SUM(E2:E32)</f>
         <v>1953</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F32)</f>
         <v>661</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="11" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="12" t="n">
+      <c r="H34" s="11" t="n">
         <f aca="false">SUM(H2:H32)</f>
         <v>1469</v>
       </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="14" t="n">
+      <c r="I34" s="12"/>
+      <c r="J34" s="13" t="n">
         <f aca="false">SUM(B34,C34,D34,E34,F34,G34,H34)</f>
         <v>13766</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="16" t="n">
+      <c r="A35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15" t="n">
         <v>1500</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="D35" s="16" t="n">
+      <c r="D35" s="15" t="n">
         <v>1500</v>
       </c>
-      <c r="E35" s="16" t="n">
+      <c r="E35" s="15" t="n">
         <v>700</v>
       </c>
-      <c r="F35" s="16" t="n">
+      <c r="F35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="15" t="n">
         <v>400</v>
       </c>
-      <c r="H35" s="16" t="n">
+      <c r="H35" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="I35" s="13"/>
-      <c r="J35" s="14" t="n">
+      <c r="I35" s="12"/>
+      <c r="J35" s="13" t="n">
         <f aca="false">SUM(B35,C35,D35,E35,F35,G35,H35)</f>
         <v>6100</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="18" t="n">
+      <c r="A36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="n">
         <f aca="false">SUM(-B34,B35)</f>
         <v>-210</v>
       </c>
-      <c r="C36" s="18" t="n">
+      <c r="C36" s="17" t="n">
         <f aca="false">SUM(-C34,C35)</f>
         <v>-6973</v>
       </c>
-      <c r="D36" s="18" t="n">
+      <c r="D36" s="17" t="n">
         <f aca="false">SUM(-D34,D35)</f>
         <v>1500</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="17" t="n">
         <f aca="false">SUM(-E34,E35)</f>
         <v>-1253</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="17" t="n">
         <f aca="false">SUM(-F34,F35)</f>
         <v>-161</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="17" t="n">
         <f aca="false">SUM(-G34,G35)</f>
         <v>400</v>
       </c>
-      <c r="H36" s="18" t="n">
+      <c r="H36" s="17" t="n">
         <f aca="false">SUM(-H34,H35)</f>
         <v>-969</v>
       </c>
-      <c r="J36" s="18" t="n">
+      <c r="J36" s="17" t="n">
         <f aca="false">SUM(B36,C36,D36,E36,F36,G36,H36)</f>
         <v>-7666</v>
       </c>

</xml_diff>